<commit_message>
Added DS - Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yashraj\Desktop\C++\competitive\DSA_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F22DB0-3A45-4BB8-9190-EA1714812E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF82777-8D90-4DF9-9B0D-4DF687A0136C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="487">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1482,7 +1482,10 @@
     <t>https://www.youtube.com/watch?v=LUm2ABqAs1w&amp;ab_channel=VivekanandKhyade-AlgorithmEveryDay</t>
   </si>
   <si>
-    <t>yes(11 or 49)</t>
+    <t>yes(11 or 49 or 50 or 51)</t>
+  </si>
+  <si>
+    <t>yes(47 or 48)</t>
   </si>
 </sst>
 </file>
@@ -2113,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15.75"/>
@@ -3871,7 +3874,7 @@
         <v>465</v>
       </c>
       <c r="E139" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="21">
@@ -3888,7 +3891,7 @@
         <v>465</v>
       </c>
       <c r="E140" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="21">
@@ -3912,129 +3915,156 @@
       <c r="A142">
         <v>50</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C142" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="D142" s="9" t="s">
-        <v>5</v>
+      <c r="D142" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E142" s="17" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="21">
       <c r="A143">
         <v>51</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C143" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D143" s="9" t="s">
-        <v>5</v>
+      <c r="D143" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E143" s="17" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="21">
       <c r="A144">
         <v>52</v>
       </c>
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C144" s="7" t="s">
+      <c r="C144" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D144" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="21">
+      <c r="D144" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E144" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="21">
       <c r="A145">
         <v>53</v>
       </c>
-      <c r="B145" s="6" t="s">
+      <c r="B145" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C145" s="7" t="s">
+      <c r="C145" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D145" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="21">
+      <c r="D145" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E145" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="21">
       <c r="A146">
         <v>54</v>
       </c>
-      <c r="B146" s="6" t="s">
+      <c r="B146" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C146" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D146" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="21">
+      <c r="D146" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E146" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="21">
       <c r="A147">
         <v>55</v>
       </c>
-      <c r="B147" s="6" t="s">
+      <c r="B147" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C147" s="7" t="s">
+      <c r="C147" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D147" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="21">
+      <c r="D147" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E147" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="21">
       <c r="A148">
         <v>56</v>
       </c>
-      <c r="B148" s="6" t="s">
+      <c r="B148" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C148" s="7" t="s">
+      <c r="C148" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D148" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="21">
+      <c r="D148" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E148" s="17" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="21">
       <c r="A149">
         <v>57</v>
       </c>
-      <c r="B149" s="6" t="s">
+      <c r="B149" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C149" s="7" t="s">
+      <c r="C149" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D149" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="21">
+      <c r="D149" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E149" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="21">
       <c r="A150">
         <v>58</v>
       </c>
-      <c r="B150" s="6" t="s">
+      <c r="B150" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C150" s="7" t="s">
+      <c r="C150" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D150" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="21">
+      <c r="D150" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="E150" s="17" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="21">
       <c r="A151">
         <v>59</v>
       </c>
@@ -4048,7 +4078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="21">
+    <row r="152" spans="1:5" ht="21">
       <c r="A152">
         <v>60</v>
       </c>
@@ -4062,7 +4092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="21">
+    <row r="153" spans="1:5" ht="21">
       <c r="A153">
         <v>61</v>
       </c>
@@ -4076,7 +4106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="21">
+    <row r="154" spans="1:5" ht="21">
       <c r="A154">
         <v>62</v>
       </c>
@@ -4090,7 +4120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="21">
+    <row r="155" spans="1:5" ht="21">
       <c r="A155">
         <v>63</v>
       </c>
@@ -4104,7 +4134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="21">
+    <row r="156" spans="1:5" ht="21">
       <c r="A156">
         <v>64</v>
       </c>
@@ -4118,7 +4148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="21">
+    <row r="157" spans="1:5" ht="21">
       <c r="A157">
         <v>65</v>
       </c>
@@ -4132,7 +4162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="21">
+    <row r="158" spans="1:5" ht="21">
       <c r="A158">
         <v>66</v>
       </c>
@@ -4146,7 +4176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="21">
+    <row r="159" spans="1:5" ht="21">
       <c r="A159">
         <v>67</v>
       </c>
@@ -4160,7 +4190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="21">
+    <row r="160" spans="1:5" ht="21">
       <c r="A160">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Added DS - Binary Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yashraj\Desktop\C++\competitive\DSA_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFFA2CD-9D8D-4902-A4DA-B0CEE42FDA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC78111-373E-4108-9E85-0F6BF881FFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="495">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1422,9 +1422,6 @@
     <t>Power Set</t>
   </si>
   <si>
-    <t>yes, correct approach</t>
-  </si>
-  <si>
     <t>KEY</t>
   </si>
   <si>
@@ -1504,6 +1501,15 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/26552481/which-is-faster-pass-by-reference-vs-pass-by-value-c</t>
+  </si>
+  <si>
+    <t>always check empty before checking first in queue or top in stack</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1436020/whats-the-difference-between-deque-and-list-stl-containers</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/print-a-binary-tree-in-vertical-order-set-3-using-level-order-traversal/</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1758,9 +1764,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2149,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15.75"/>
@@ -2174,12 +2177,12 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="F3" s="16" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21">
@@ -2193,10 +2196,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2213,10 +2216,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21">
@@ -2230,10 +2233,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21">
@@ -2247,10 +2250,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21">
@@ -2264,10 +2267,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21">
@@ -2281,10 +2284,10 @@
         <v>11</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
@@ -2298,10 +2301,10 @@
         <v>12</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21">
@@ -2315,10 +2318,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21">
@@ -2332,10 +2335,10 @@
         <v>14</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E13" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
@@ -2349,10 +2352,10 @@
         <v>15</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21">
@@ -2362,14 +2365,14 @@
       <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21">
@@ -2383,13 +2386,13 @@
         <v>17</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F16" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21">
@@ -2403,10 +2406,10 @@
         <v>18</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21">
@@ -2420,10 +2423,10 @@
         <v>19</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21">
@@ -2437,10 +2440,10 @@
         <v>20</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21">
@@ -2454,10 +2457,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21">
@@ -2471,10 +2474,10 @@
         <v>22</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E21" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21">
@@ -2488,10 +2491,10 @@
         <v>23</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="21">
@@ -2505,10 +2508,10 @@
         <v>24</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21">
@@ -2522,10 +2525,10 @@
         <v>25</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21">
@@ -2539,10 +2542,10 @@
         <v>26</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21">
@@ -2556,10 +2559,10 @@
         <v>27</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21">
@@ -2573,10 +2576,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21">
@@ -2590,10 +2593,10 @@
         <v>29</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21">
@@ -2607,10 +2610,10 @@
         <v>30</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="21">
@@ -2624,10 +2627,10 @@
         <v>31</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="21">
@@ -2641,10 +2644,10 @@
         <v>32</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E31" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="21">
@@ -2658,10 +2661,10 @@
         <v>33</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E32" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="21">
@@ -2675,10 +2678,10 @@
         <v>34</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="21">
@@ -2692,10 +2695,10 @@
         <v>35</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E34" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="21">
@@ -2709,10 +2712,10 @@
         <v>36</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E35" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="21">
@@ -2726,10 +2729,10 @@
         <v>37</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E36" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="21">
@@ -2743,10 +2746,10 @@
         <v>38</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E37" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="21">
@@ -2760,10 +2763,10 @@
         <v>39</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="21">
@@ -2777,13 +2780,13 @@
         <v>40</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="21">
@@ -2797,13 +2800,13 @@
         <v>41</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E40" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F40" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="21">
@@ -2817,10 +2820,10 @@
         <v>42</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="21">
@@ -2847,10 +2850,10 @@
         <v>44</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="21">
@@ -2864,10 +2867,10 @@
         <v>45</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E45" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -2881,10 +2884,10 @@
         <v>46</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E46" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="21">
@@ -2898,10 +2901,10 @@
         <v>47</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E47" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -2915,10 +2918,10 @@
         <v>48</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E48" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="21">
@@ -2932,10 +2935,10 @@
         <v>49</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E49" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="21">
@@ -2949,10 +2952,10 @@
         <v>50</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E50" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21">
@@ -2966,13 +2969,13 @@
         <v>51</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E51" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F51" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="21">
@@ -2986,10 +2989,10 @@
         <v>52</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E52" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="21">
@@ -3003,10 +3006,10 @@
         <v>53</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E53" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="21">
@@ -3906,10 +3909,10 @@
         <v>136</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E139" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="21">
@@ -3923,10 +3926,10 @@
         <v>137</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E140" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="21">
@@ -3940,10 +3943,10 @@
         <v>138</v>
       </c>
       <c r="D141" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="21">
@@ -3957,10 +3960,10 @@
         <v>139</v>
       </c>
       <c r="D142" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E142" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="21">
@@ -3974,10 +3977,10 @@
         <v>140</v>
       </c>
       <c r="D143" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E143" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="21">
@@ -3991,10 +3994,10 @@
         <v>141</v>
       </c>
       <c r="D144" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E144" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="21">
@@ -4008,10 +4011,10 @@
         <v>142</v>
       </c>
       <c r="D145" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E145" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="21">
@@ -4025,10 +4028,10 @@
         <v>143</v>
       </c>
       <c r="D146" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E146" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="21">
@@ -4042,10 +4045,10 @@
         <v>144</v>
       </c>
       <c r="D147" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E147" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="21">
@@ -4059,10 +4062,10 @@
         <v>145</v>
       </c>
       <c r="D148" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E148" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="21">
@@ -4076,10 +4079,10 @@
         <v>146</v>
       </c>
       <c r="D149" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E149" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="21">
@@ -4093,10 +4096,10 @@
         <v>147</v>
       </c>
       <c r="D150" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E150" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="21">
@@ -4110,10 +4113,10 @@
         <v>148</v>
       </c>
       <c r="D151" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E151" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="21">
@@ -4127,10 +4130,10 @@
         <v>149</v>
       </c>
       <c r="D152" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E152" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="21">
@@ -4144,10 +4147,10 @@
         <v>150</v>
       </c>
       <c r="D153" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E153" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="21">
@@ -4161,10 +4164,10 @@
         <v>151</v>
       </c>
       <c r="D154" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E154" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="21">
@@ -4178,10 +4181,10 @@
         <v>152</v>
       </c>
       <c r="D155" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E155" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="21">
@@ -4195,10 +4198,10 @@
         <v>153</v>
       </c>
       <c r="D156" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E156" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="21">
@@ -4212,10 +4215,10 @@
         <v>154</v>
       </c>
       <c r="D157" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E157" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="21">
@@ -4229,10 +4232,10 @@
         <v>155</v>
       </c>
       <c r="D158" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E158" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="21">
@@ -4246,10 +4249,10 @@
         <v>156</v>
       </c>
       <c r="D159" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E159" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="21">
@@ -4263,10 +4266,10 @@
         <v>157</v>
       </c>
       <c r="D160" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E160" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="21">
@@ -4280,13 +4283,13 @@
         <v>158</v>
       </c>
       <c r="D161" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E161" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F161" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="21">
@@ -4300,10 +4303,10 @@
         <v>159</v>
       </c>
       <c r="D162" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E162" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="21">
@@ -4317,10 +4320,10 @@
         <v>160</v>
       </c>
       <c r="D163" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E163" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="21">
@@ -4334,13 +4337,13 @@
         <v>161</v>
       </c>
       <c r="D164" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E164" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F164" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="21">
@@ -4354,13 +4357,13 @@
         <v>162</v>
       </c>
       <c r="D165" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E165" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F165" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="21">
@@ -4374,10 +4377,10 @@
         <v>163</v>
       </c>
       <c r="D166" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E166" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="21">
@@ -4391,10 +4394,10 @@
         <v>164</v>
       </c>
       <c r="D167" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E167" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="21">
@@ -4408,10 +4411,10 @@
         <v>165</v>
       </c>
       <c r="D168" s="30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E168" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="21">
@@ -4425,10 +4428,10 @@
         <v>166</v>
       </c>
       <c r="D169" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E169" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="21">
@@ -4442,10 +4445,10 @@
         <v>167</v>
       </c>
       <c r="D170" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E170" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="21">
@@ -4459,10 +4462,10 @@
         <v>168</v>
       </c>
       <c r="D171" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E171" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="21">
@@ -4476,10 +4479,10 @@
         <v>169</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E172" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="21">
@@ -4493,10 +4496,10 @@
         <v>170</v>
       </c>
       <c r="D173" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E173" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="21">
@@ -4510,149 +4513,227 @@
         <v>171</v>
       </c>
       <c r="D174" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E174" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="21">
       <c r="C176" s="8"/>
       <c r="D176" s="9"/>
     </row>
-    <row r="177" spans="2:4" ht="21">
-      <c r="B177" s="6" t="s">
+    <row r="177" spans="1:6" ht="21">
+      <c r="A177">
+        <v>121</v>
+      </c>
+      <c r="B177" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C177" s="7" t="s">
+      <c r="C177" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="D177" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" ht="21">
-      <c r="B178" s="6" t="s">
+      <c r="D177" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E177" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="21">
+      <c r="A178">
+        <v>122</v>
+      </c>
+      <c r="B178" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C178" s="7" t="s">
+      <c r="C178" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="D178" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" ht="21">
-      <c r="B179" s="6" t="s">
+      <c r="D178" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E178" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="21">
+      <c r="A179">
+        <v>123</v>
+      </c>
+      <c r="B179" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C179" s="7" t="s">
+      <c r="C179" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="D179" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" ht="21">
-      <c r="B180" s="6" t="s">
+      <c r="D179" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E179" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="21">
+      <c r="A180">
+        <v>124</v>
+      </c>
+      <c r="B180" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C180" s="7" t="s">
+      <c r="C180" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="D180" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" ht="21">
-      <c r="B181" s="6" t="s">
+      <c r="D180" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E180" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="21">
+      <c r="A181">
+        <v>125</v>
+      </c>
+      <c r="B181" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C181" s="7" t="s">
+      <c r="C181" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="D181" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4" ht="21">
-      <c r="B182" s="6" t="s">
+      <c r="D181" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E181" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="21">
+      <c r="A182">
+        <v>126</v>
+      </c>
+      <c r="B182" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C182" s="7" t="s">
+      <c r="C182" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D182" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" ht="21">
-      <c r="B183" s="6" t="s">
+      <c r="D182" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E182" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="21">
+      <c r="A183">
+        <v>127</v>
+      </c>
+      <c r="B183" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C183" s="7" t="s">
+      <c r="C183" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="D183" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" ht="21">
-      <c r="B184" s="6" t="s">
+      <c r="D183" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E183" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="21">
+      <c r="A184">
+        <v>128</v>
+      </c>
+      <c r="B184" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C184" s="7" t="s">
+      <c r="C184" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="D184" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="185" spans="2:4" ht="21">
-      <c r="B185" s="6" t="s">
+      <c r="D184" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E184" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" ht="21">
+      <c r="A185">
+        <v>129</v>
+      </c>
+      <c r="B185" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C185" s="7" t="s">
+      <c r="C185" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D185" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" spans="2:4" ht="21">
-      <c r="B186" s="6" t="s">
+      <c r="D185" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E185" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" ht="21">
+      <c r="A186">
+        <v>130</v>
+      </c>
+      <c r="B186" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C186" s="7" t="s">
+      <c r="C186" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D186" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="2:4" ht="21">
-      <c r="B187" s="6" t="s">
+      <c r="D186" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E186" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" ht="21">
+      <c r="A187">
+        <v>131</v>
+      </c>
+      <c r="B187" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C187" s="7" t="s">
+      <c r="C187" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="D187" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" spans="2:4" ht="21">
-      <c r="B188" s="6" t="s">
+      <c r="D187" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E187" t="s">
+        <v>467</v>
+      </c>
+      <c r="F187" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" ht="21">
+      <c r="A188">
+        <v>132</v>
+      </c>
+      <c r="B188" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C188" s="7" t="s">
+      <c r="C188" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="D188" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="189" spans="2:4" ht="21">
+      <c r="D188" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E188" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" ht="21">
+      <c r="A189">
+        <v>133</v>
+      </c>
       <c r="B189" s="6" t="s">
         <v>172</v>
       </c>
@@ -4663,7 +4744,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="2:4" ht="21">
+    <row r="190" spans="1:6" ht="21">
+      <c r="A190">
+        <v>134</v>
+      </c>
       <c r="B190" s="6" t="s">
         <v>172</v>
       </c>
@@ -4674,7 +4758,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="2:4" ht="21">
+    <row r="191" spans="1:6" ht="21">
+      <c r="A191">
+        <v>135</v>
+      </c>
       <c r="B191" s="6" t="s">
         <v>172</v>
       </c>
@@ -4685,7 +4772,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="2:4" ht="21">
+    <row r="192" spans="1:6" ht="21">
+      <c r="A192">
+        <v>136</v>
+      </c>
       <c r="B192" s="6" t="s">
         <v>172</v>
       </c>
@@ -4696,7 +4786,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="21">
+    <row r="193" spans="1:4" ht="21">
+      <c r="A193">
+        <v>137</v>
+      </c>
       <c r="B193" s="6" t="s">
         <v>172</v>
       </c>
@@ -4707,7 +4800,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="2:4" ht="21">
+    <row r="194" spans="1:4" ht="21">
+      <c r="A194">
+        <v>138</v>
+      </c>
       <c r="B194" s="6" t="s">
         <v>172</v>
       </c>
@@ -4718,7 +4814,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="2:4" ht="21">
+    <row r="195" spans="1:4" ht="21">
+      <c r="A195">
+        <v>139</v>
+      </c>
       <c r="B195" s="6" t="s">
         <v>172</v>
       </c>
@@ -4729,7 +4828,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="2:4" ht="21">
+    <row r="196" spans="1:4" ht="21">
+      <c r="A196">
+        <v>140</v>
+      </c>
       <c r="B196" s="6" t="s">
         <v>172</v>
       </c>
@@ -4740,7 +4842,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="2:4" ht="21">
+    <row r="197" spans="1:4" ht="21">
+      <c r="A197">
+        <v>141</v>
+      </c>
       <c r="B197" s="6" t="s">
         <v>172</v>
       </c>
@@ -4751,7 +4856,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="2:4" ht="21">
+    <row r="198" spans="1:4" ht="21">
+      <c r="A198">
+        <v>142</v>
+      </c>
       <c r="B198" s="6" t="s">
         <v>172</v>
       </c>
@@ -4762,7 +4870,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="2:4" ht="21">
+    <row r="199" spans="1:4" ht="21">
+      <c r="A199">
+        <v>143</v>
+      </c>
       <c r="B199" s="6" t="s">
         <v>172</v>
       </c>
@@ -4773,7 +4884,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="2:4" ht="21">
+    <row r="200" spans="1:4" ht="21">
+      <c r="A200">
+        <v>144</v>
+      </c>
       <c r="B200" s="6" t="s">
         <v>172</v>
       </c>
@@ -4784,7 +4898,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="2:4" ht="21">
+    <row r="201" spans="1:4" ht="21">
+      <c r="A201">
+        <v>145</v>
+      </c>
       <c r="B201" s="6" t="s">
         <v>172</v>
       </c>
@@ -4795,7 +4912,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="2:4" ht="21">
+    <row r="202" spans="1:4" ht="21">
+      <c r="A202">
+        <v>146</v>
+      </c>
       <c r="B202" s="6" t="s">
         <v>172</v>
       </c>
@@ -4806,7 +4926,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="2:4" ht="21">
+    <row r="203" spans="1:4" ht="21">
+      <c r="A203">
+        <v>147</v>
+      </c>
       <c r="B203" s="6" t="s">
         <v>172</v>
       </c>
@@ -4817,7 +4940,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="2:4" ht="21">
+    <row r="204" spans="1:4" ht="21">
+      <c r="A204">
+        <v>148</v>
+      </c>
       <c r="B204" s="6" t="s">
         <v>172</v>
       </c>
@@ -4828,7 +4954,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="2:4" ht="21">
+    <row r="205" spans="1:4" ht="21">
+      <c r="A205">
+        <v>149</v>
+      </c>
       <c r="B205" s="6" t="s">
         <v>172</v>
       </c>
@@ -4839,7 +4968,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="2:4" ht="21">
+    <row r="206" spans="1:4" ht="21">
+      <c r="A206">
+        <v>150</v>
+      </c>
       <c r="B206" s="6" t="s">
         <v>172</v>
       </c>
@@ -4850,7 +4982,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="2:4" ht="21">
+    <row r="207" spans="1:4" ht="21">
+      <c r="A207">
+        <v>151</v>
+      </c>
       <c r="B207" s="6" t="s">
         <v>172</v>
       </c>
@@ -4861,7 +4996,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="2:4" ht="21">
+    <row r="208" spans="1:4" ht="21">
+      <c r="A208">
+        <v>152</v>
+      </c>
       <c r="B208" s="6" t="s">
         <v>172</v>
       </c>
@@ -4872,7 +5010,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="2:4" ht="21">
+    <row r="209" spans="1:4" ht="21">
+      <c r="A209">
+        <v>153</v>
+      </c>
       <c r="B209" s="6" t="s">
         <v>172</v>
       </c>
@@ -4883,7 +5024,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="2:4" ht="21">
+    <row r="210" spans="1:4" ht="21">
+      <c r="A210">
+        <v>154</v>
+      </c>
       <c r="B210" s="6" t="s">
         <v>172</v>
       </c>
@@ -4894,7 +5038,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="2:4" ht="21">
+    <row r="211" spans="1:4" ht="21">
+      <c r="A211">
+        <v>155</v>
+      </c>
       <c r="B211" s="6" t="s">
         <v>172</v>
       </c>
@@ -4905,17 +5052,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="2:4" ht="21">
+    <row r="212" spans="1:4" ht="21">
       <c r="B212" s="6"/>
       <c r="C212" s="8"/>
       <c r="D212" s="9"/>
     </row>
-    <row r="213" spans="2:4" ht="21">
+    <row r="213" spans="1:4" ht="21">
       <c r="B213" s="6"/>
       <c r="C213" s="8"/>
       <c r="D213" s="9"/>
     </row>
-    <row r="214" spans="2:4" ht="21">
+    <row r="214" spans="1:4" ht="21">
       <c r="B214" s="6" t="s">
         <v>208</v>
       </c>
@@ -4926,7 +5073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="2:4" ht="21">
+    <row r="215" spans="1:4" ht="21">
       <c r="B215" s="6" t="s">
         <v>208</v>
       </c>
@@ -4937,7 +5084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="2:4" ht="21">
+    <row r="216" spans="1:4" ht="21">
       <c r="B216" s="6" t="s">
         <v>208</v>
       </c>
@@ -4948,7 +5095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="2:4" ht="21">
+    <row r="217" spans="1:4" ht="21">
       <c r="B217" s="6" t="s">
         <v>208</v>
       </c>
@@ -4959,7 +5106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="2:4" ht="21">
+    <row r="218" spans="1:4" ht="21">
       <c r="B218" s="6" t="s">
         <v>208</v>
       </c>
@@ -4970,7 +5117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="2:4" ht="21">
+    <row r="219" spans="1:4" ht="21">
       <c r="B219" s="6" t="s">
         <v>208</v>
       </c>
@@ -4981,7 +5128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:4" ht="21">
+    <row r="220" spans="1:4" ht="21">
       <c r="B220" s="6" t="s">
         <v>208</v>
       </c>
@@ -4992,7 +5139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="2:4" ht="21">
+    <row r="221" spans="1:4" ht="21">
       <c r="B221" s="6" t="s">
         <v>208</v>
       </c>
@@ -5003,7 +5150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="2:4" ht="21">
+    <row r="222" spans="1:4" ht="21">
       <c r="B222" s="6" t="s">
         <v>208</v>
       </c>
@@ -5014,7 +5161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="2:4" ht="21">
+    <row r="223" spans="1:4" ht="21">
       <c r="B223" s="6" t="s">
         <v>208</v>
       </c>
@@ -5025,7 +5172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="2:4" ht="21">
+    <row r="224" spans="1:4" ht="21">
       <c r="B224" s="6" t="s">
         <v>208</v>
       </c>
@@ -5786,10 +5933,10 @@
         <v>287</v>
       </c>
       <c r="D296" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E296" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="21">
@@ -5803,10 +5950,10 @@
         <v>288</v>
       </c>
       <c r="D297" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E297" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="21">
@@ -5820,10 +5967,10 @@
         <v>289</v>
       </c>
       <c r="D298" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E298" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="21">
@@ -5837,10 +5984,10 @@
         <v>290</v>
       </c>
       <c r="D299" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E299" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="21">
@@ -5854,10 +6001,10 @@
         <v>291</v>
       </c>
       <c r="D300" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E300" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="301" spans="1:6" ht="21">
@@ -5871,10 +6018,10 @@
         <v>292</v>
       </c>
       <c r="D301" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E301" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="21">
@@ -5888,10 +6035,10 @@
         <v>293</v>
       </c>
       <c r="D302" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E302" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="21">
@@ -5905,13 +6052,13 @@
         <v>294</v>
       </c>
       <c r="D303" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E303" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F303" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="21">
@@ -5925,10 +6072,10 @@
         <v>295</v>
       </c>
       <c r="D304" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E304" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="21">
@@ -5942,10 +6089,10 @@
         <v>296</v>
       </c>
       <c r="D305" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E305" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="21">
@@ -5959,13 +6106,13 @@
         <v>297</v>
       </c>
       <c r="D306" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E306" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F306" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="21">
@@ -5979,10 +6126,10 @@
         <v>298</v>
       </c>
       <c r="D307" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E307" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="21">
@@ -5996,10 +6143,10 @@
         <v>299</v>
       </c>
       <c r="D308" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E308" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="309" spans="1:6" ht="21">
@@ -6013,10 +6160,10 @@
         <v>300</v>
       </c>
       <c r="D309" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E309" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="310" spans="1:6" ht="21">
@@ -6030,10 +6177,10 @@
         <v>301</v>
       </c>
       <c r="D310" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E310" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="21">
@@ -6047,10 +6194,10 @@
         <v>302</v>
       </c>
       <c r="D311" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E311" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6064,10 +6211,10 @@
         <v>303</v>
       </c>
       <c r="D312" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E312" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="313" spans="1:6" ht="21">
@@ -6081,10 +6228,10 @@
         <v>304</v>
       </c>
       <c r="D313" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E313" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F313" s="17"/>
     </row>
@@ -6099,10 +6246,10 @@
         <v>305</v>
       </c>
       <c r="D314" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E314" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F314" s="17"/>
     </row>
@@ -6117,10 +6264,10 @@
         <v>306</v>
       </c>
       <c r="D315" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E315" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F315" s="17"/>
     </row>
@@ -6135,12 +6282,14 @@
         <v>307</v>
       </c>
       <c r="D316" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E316" t="s">
-        <v>469</v>
-      </c>
-      <c r="F316" s="17"/>
+        <v>468</v>
+      </c>
+      <c r="F316" s="17" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="317" spans="1:6" ht="21">
       <c r="A317">
@@ -6153,10 +6302,10 @@
         <v>308</v>
       </c>
       <c r="D317" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E317" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F317" s="17"/>
     </row>
@@ -6171,10 +6320,10 @@
         <v>309</v>
       </c>
       <c r="D318" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E318" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F318" s="17"/>
     </row>
@@ -6189,10 +6338,10 @@
         <v>310</v>
       </c>
       <c r="D319" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E319" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F319" s="17"/>
     </row>
@@ -6207,10 +6356,10 @@
         <v>311</v>
       </c>
       <c r="D320" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E320" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F320" s="17"/>
     </row>
@@ -6218,17 +6367,17 @@
       <c r="A321">
         <v>108</v>
       </c>
-      <c r="B321" s="23" t="s">
+      <c r="B321" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C321" s="26" t="s">
+      <c r="C321" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="D321" s="34" t="s">
-        <v>476</v>
+      <c r="D321" s="25" t="s">
+        <v>467</v>
       </c>
       <c r="E321" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F321" s="17"/>
     </row>
@@ -6243,13 +6392,13 @@
         <v>313</v>
       </c>
       <c r="D322" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E322" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F322" s="17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="21">
@@ -6263,10 +6412,10 @@
         <v>314</v>
       </c>
       <c r="D323" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E323" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F323" s="17"/>
     </row>
@@ -6281,10 +6430,10 @@
         <v>315</v>
       </c>
       <c r="D324" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E324" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F324" s="17"/>
     </row>
@@ -6299,12 +6448,12 @@
         <v>316</v>
       </c>
       <c r="D325" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E325" t="s">
-        <v>468</v>
-      </c>
-      <c r="F325" s="36"/>
+        <v>467</v>
+      </c>
+      <c r="F325" s="35"/>
     </row>
     <row r="326" spans="1:6" ht="21">
       <c r="A326">
@@ -6317,10 +6466,10 @@
         <v>317</v>
       </c>
       <c r="D326" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E326" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="21">
@@ -6334,94 +6483,115 @@
         <v>318</v>
       </c>
       <c r="D327" s="25" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E327" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328">
         <v>115</v>
       </c>
-      <c r="B328" s="6" t="s">
+      <c r="B328" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C328" s="7" t="s">
+      <c r="C328" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="D328" s="9" t="s">
-        <v>5</v>
+      <c r="D328" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E328" t="s">
+        <v>467</v>
+      </c>
+      <c r="F328" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="21">
       <c r="A329">
         <v>116</v>
       </c>
-      <c r="B329" s="6" t="s">
+      <c r="B329" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C329" s="7" t="s">
+      <c r="C329" s="27" t="s">
         <v>320</v>
       </c>
-      <c r="D329" s="9" t="s">
-        <v>5</v>
+      <c r="D329" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E329" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="330" spans="1:6" ht="21">
       <c r="A330">
         <v>117</v>
       </c>
-      <c r="B330" s="6" t="s">
+      <c r="B330" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C330" s="7" t="s">
+      <c r="C330" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="D330" s="9" t="s">
-        <v>5</v>
+      <c r="D330" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E330" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331">
         <v>118</v>
       </c>
-      <c r="B331" s="6" t="s">
+      <c r="B331" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="C331" s="7" t="s">
+      <c r="C331" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="D331" s="9" t="s">
-        <v>5</v>
+      <c r="D331" s="24" t="s">
+        <v>474</v>
+      </c>
+      <c r="E331" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="21">
       <c r="A332">
         <v>119</v>
       </c>
-      <c r="B332" s="6" t="s">
+      <c r="B332" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C332" s="7" t="s">
+      <c r="C332" s="27" t="s">
         <v>323</v>
       </c>
-      <c r="D332" s="9" t="s">
-        <v>5</v>
+      <c r="D332" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E332" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="333" spans="1:6" ht="21">
       <c r="A333">
         <v>120</v>
       </c>
-      <c r="B333" s="6" t="s">
+      <c r="B333" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="C333" s="7" t="s">
+      <c r="C333" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="D333" s="9" t="s">
-        <v>5</v>
+      <c r="D333" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E333" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="334" spans="1:6" ht="21">

</xml_diff>

<commit_message>
Added DS - Binary Search Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yashraj\Desktop\C++\competitive\DSA_Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3E7CF3-34C0-47C7-8475-B9D87172BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CDFBF0-7AF4-4E48-9141-457B44A83B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="500">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1513,6 +1513,18 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/minimum-number-swaps-required-sort-array/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/avl-tree-set-1-insertion/</t>
+  </si>
+  <si>
+    <t>links in comments in code</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/inorder-tree-traversal-without-recursion-and-without-stack/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wGXB9OWhPTg&amp;ab_channel=TusharRoy-CodingMadeSimple</t>
   </si>
 </sst>
 </file>
@@ -1706,7 +1718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1781,6 +1793,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2166,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B197" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C207" sqref="C207"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B230" sqref="B230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15.75"/>
@@ -2405,7 +2418,7 @@
       <c r="E16" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="38" t="s">
         <v>483</v>
       </c>
     </row>
@@ -2493,7 +2506,7 @@
       <c r="E21" t="s">
         <v>467</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="38" t="s">
         <v>495</v>
       </c>
     </row>
@@ -2802,7 +2815,7 @@
       <c r="E39" t="s">
         <v>480</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="38" t="s">
         <v>478</v>
       </c>
     </row>
@@ -2822,7 +2835,7 @@
       <c r="E40" t="s">
         <v>481</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="38" t="s">
         <v>479</v>
       </c>
     </row>
@@ -2991,7 +3004,7 @@
       <c r="E51" t="s">
         <v>467</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="38" t="s">
         <v>482</v>
       </c>
     </row>
@@ -4305,7 +4318,7 @@
       <c r="E161" t="s">
         <v>467</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F161" s="38" t="s">
         <v>486</v>
       </c>
     </row>
@@ -4359,7 +4372,7 @@
       <c r="E164" t="s">
         <v>467</v>
       </c>
-      <c r="F164" t="s">
+      <c r="F164" s="38" t="s">
         <v>487</v>
       </c>
     </row>
@@ -4379,7 +4392,7 @@
       <c r="E165" t="s">
         <v>467</v>
       </c>
-      <c r="F165" t="s">
+      <c r="F165" s="38" t="s">
         <v>488</v>
       </c>
     </row>
@@ -4641,6 +4654,9 @@
       <c r="E182" t="s">
         <v>467</v>
       </c>
+      <c r="F182" s="38" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="183" spans="1:6" ht="21">
       <c r="A183">
@@ -4726,7 +4742,7 @@
       <c r="E187" t="s">
         <v>467</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" s="38" t="s">
         <v>494</v>
       </c>
     </row>
@@ -5074,256 +5090,382 @@
       <c r="A208">
         <v>152</v>
       </c>
-      <c r="B208" s="6" t="s">
+      <c r="B208" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C208" s="7" t="s">
+      <c r="C208" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="D208" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" ht="21">
+      <c r="D208" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E208" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="21">
       <c r="A209">
         <v>153</v>
       </c>
-      <c r="B209" s="6" t="s">
+      <c r="B209" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C209" s="7" t="s">
+      <c r="C209" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="D209" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" ht="21">
+      <c r="D209" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E209" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" ht="21">
       <c r="A210">
         <v>154</v>
       </c>
-      <c r="B210" s="6" t="s">
+      <c r="B210" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C210" s="7" t="s">
+      <c r="C210" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="D210" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" ht="21">
+      <c r="D210" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E210" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" ht="21">
       <c r="A211">
         <v>155</v>
       </c>
-      <c r="B211" s="6" t="s">
+      <c r="B211" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C211" s="7" t="s">
+      <c r="C211" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="D211" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" ht="21">
+      <c r="D211" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E211" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="21">
       <c r="B212" s="6"/>
       <c r="C212" s="8"/>
       <c r="D212" s="9"/>
     </row>
-    <row r="213" spans="1:4" ht="21">
+    <row r="213" spans="1:6" ht="21">
       <c r="B213" s="6"/>
       <c r="C213" s="8"/>
       <c r="D213" s="9"/>
     </row>
-    <row r="214" spans="1:4" ht="21">
-      <c r="B214" s="6" t="s">
+    <row r="214" spans="1:6" ht="21">
+      <c r="A214">
+        <v>156</v>
+      </c>
+      <c r="B214" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C214" s="7" t="s">
+      <c r="C214" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="D214" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" ht="21">
-      <c r="B215" s="6" t="s">
+      <c r="D214" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E214" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="21">
+      <c r="A215">
+        <v>157</v>
+      </c>
+      <c r="B215" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C215" s="7" t="s">
+      <c r="C215" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="D215" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" ht="21">
-      <c r="B216" s="6" t="s">
+      <c r="D215" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E215" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" ht="21">
+      <c r="A216">
+        <v>158</v>
+      </c>
+      <c r="B216" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C216" s="7" t="s">
+      <c r="C216" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="D216" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" ht="21">
-      <c r="B217" s="6" t="s">
+      <c r="D216" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E216" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="21">
+      <c r="A217">
+        <v>159</v>
+      </c>
+      <c r="B217" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C217" s="7" t="s">
+      <c r="C217" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="D217" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" ht="21">
-      <c r="B218" s="6" t="s">
+      <c r="D217" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E217" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" ht="21">
+      <c r="A218">
+        <v>160</v>
+      </c>
+      <c r="B218" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C218" s="7" t="s">
+      <c r="C218" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="D218" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" ht="21">
-      <c r="B219" s="6" t="s">
+      <c r="D218" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E218" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="21">
+      <c r="A219">
+        <v>161</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C219" s="7" t="s">
+      <c r="C219" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="D219" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" ht="21">
-      <c r="B220" s="6" t="s">
+      <c r="D219" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E219" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="21">
+      <c r="A220">
+        <v>162</v>
+      </c>
+      <c r="B220" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C220" s="10" t="s">
+      <c r="C220" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="D220" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" ht="21">
-      <c r="B221" s="6" t="s">
+      <c r="D220" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E220" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="21">
+      <c r="A221">
+        <v>163</v>
+      </c>
+      <c r="B221" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C221" s="7" t="s">
+      <c r="C221" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="D221" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" ht="21">
-      <c r="B222" s="6" t="s">
+      <c r="D221" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E221" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="21">
+      <c r="A222">
+        <v>164</v>
+      </c>
+      <c r="B222" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C222" s="7" t="s">
+      <c r="C222" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="D222" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" ht="21">
-      <c r="B223" s="6" t="s">
+      <c r="D222" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E222" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="21">
+      <c r="A223">
+        <v>165</v>
+      </c>
+      <c r="B223" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C223" s="7" t="s">
+      <c r="C223" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="D223" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" ht="21">
-      <c r="B224" s="6" t="s">
+      <c r="D223" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E223" t="s">
+        <v>467</v>
+      </c>
+      <c r="F223" s="38" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="21">
+      <c r="A224">
+        <v>166</v>
+      </c>
+      <c r="B224" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C224" s="7" t="s">
+      <c r="C224" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="D224" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="225" spans="2:4" ht="21">
-      <c r="B225" s="6" t="s">
+      <c r="D224" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E224" t="s">
+        <v>467</v>
+      </c>
+      <c r="F224" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="21">
+      <c r="A225">
+        <v>167</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C225" s="7" t="s">
+      <c r="C225" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="D225" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="226" spans="2:4" ht="21">
-      <c r="B226" s="6" t="s">
+      <c r="D225" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E225" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="21">
+      <c r="A226">
+        <v>168</v>
+      </c>
+      <c r="B226" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C226" s="7" t="s">
+      <c r="C226" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="D226" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="227" spans="2:4" ht="21">
-      <c r="B227" s="6" t="s">
+      <c r="D226" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E226" t="s">
+        <v>467</v>
+      </c>
+      <c r="F226" s="38" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="21">
+      <c r="A227">
+        <v>169</v>
+      </c>
+      <c r="B227" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C227" s="7" t="s">
+      <c r="C227" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="D227" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="228" spans="2:4" ht="21">
-      <c r="B228" s="6" t="s">
+      <c r="D227" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E227" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="21">
+      <c r="A228">
+        <v>170</v>
+      </c>
+      <c r="B228" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C228" s="7" t="s">
+      <c r="C228" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="D228" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="229" spans="2:4" ht="21">
-      <c r="B229" s="6" t="s">
+      <c r="D228" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E228" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="21">
+      <c r="A229">
+        <v>171</v>
+      </c>
+      <c r="B229" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C229" s="7" t="s">
+      <c r="C229" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="D229" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="230" spans="2:4" ht="21">
-      <c r="B230" s="6" t="s">
+      <c r="D229" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E229" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="21">
+      <c r="A230">
+        <v>172</v>
+      </c>
+      <c r="B230" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C230" s="7" t="s">
+      <c r="C230" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="D230" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="231" spans="2:4" ht="21">
+      <c r="D230" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E230" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="21">
+      <c r="A231">
+        <v>173</v>
+      </c>
       <c r="B231" s="6" t="s">
         <v>208</v>
       </c>
@@ -5334,7 +5476,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="2:4" ht="21">
+    <row r="232" spans="1:6" ht="21">
+      <c r="A232">
+        <v>174</v>
+      </c>
       <c r="B232" s="6" t="s">
         <v>208</v>
       </c>
@@ -5345,7 +5490,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="2:4" ht="21">
+    <row r="233" spans="1:6" ht="21">
+      <c r="A233">
+        <v>175</v>
+      </c>
       <c r="B233" s="6" t="s">
         <v>208</v>
       </c>
@@ -5356,7 +5504,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="2:4" ht="21">
+    <row r="234" spans="1:6" ht="21">
+      <c r="A234">
+        <v>176</v>
+      </c>
       <c r="B234" s="6" t="s">
         <v>208</v>
       </c>
@@ -5367,7 +5518,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="2:4" ht="21">
+    <row r="235" spans="1:6" ht="21">
+      <c r="A235">
+        <v>177</v>
+      </c>
       <c r="B235" s="6" t="s">
         <v>208</v>
       </c>
@@ -5378,15 +5532,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="2:4" ht="21">
+    <row r="236" spans="1:6" ht="21">
       <c r="C236" s="8"/>
       <c r="D236" s="9"/>
     </row>
-    <row r="237" spans="2:4" ht="21">
+    <row r="237" spans="1:6" ht="21">
       <c r="C237" s="8"/>
       <c r="D237" s="9"/>
     </row>
-    <row r="238" spans="2:4" ht="21">
+    <row r="238" spans="1:6" ht="21">
       <c r="B238" s="6" t="s">
         <v>231</v>
       </c>
@@ -5397,7 +5551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="2:4" ht="21">
+    <row r="239" spans="1:6" ht="21">
       <c r="B239" s="6" t="s">
         <v>231</v>
       </c>
@@ -5408,7 +5562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="2:4" ht="21">
+    <row r="240" spans="1:6" ht="21">
       <c r="B240" s="6" t="s">
         <v>231</v>
       </c>
@@ -6131,7 +6285,7 @@
       <c r="E303" t="s">
         <v>467</v>
       </c>
-      <c r="F303" t="s">
+      <c r="F303" s="38" t="s">
         <v>489</v>
       </c>
     </row>
@@ -6185,7 +6339,7 @@
       <c r="E306" t="s">
         <v>467</v>
       </c>
-      <c r="F306" t="s">
+      <c r="F306" s="38" t="s">
         <v>490</v>
       </c>
     </row>
@@ -6361,7 +6515,7 @@
       <c r="E316" t="s">
         <v>468</v>
       </c>
-      <c r="F316" s="17" t="s">
+      <c r="F316" s="38" t="s">
         <v>493</v>
       </c>
     </row>
@@ -6471,7 +6625,7 @@
       <c r="E322" t="s">
         <v>468</v>
       </c>
-      <c r="F322" s="17" t="s">
+      <c r="F322" s="38" t="s">
         <v>491</v>
       </c>
     </row>
@@ -8675,8 +8829,23 @@
     <hyperlink ref="C481" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
     <hyperlink ref="C206" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
     <hyperlink ref="C205" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="F187" r:id="rId447" xr:uid="{EE53B277-205C-4364-B4AC-A4C21D47A22E}"/>
+    <hyperlink ref="F182" r:id="rId448" xr:uid="{F3F1152E-FF97-49CD-BF76-50FD8BFC91CE}"/>
+    <hyperlink ref="F223" r:id="rId449" xr:uid="{DD98D22B-3F36-4AED-A589-27275A914741}"/>
+    <hyperlink ref="F165" r:id="rId450" xr:uid="{0A34F150-FA9C-48BA-995D-F3E43C20F37F}"/>
+    <hyperlink ref="F164" r:id="rId451" xr:uid="{49CA8565-971B-421A-B4BA-8379711B1849}"/>
+    <hyperlink ref="F161" r:id="rId452" xr:uid="{EB09B99E-4109-4462-8E1E-F7301883DF8C}"/>
+    <hyperlink ref="F51" r:id="rId453" xr:uid="{39B5B4EF-EC99-41BC-B94E-1B1BE1B236CD}"/>
+    <hyperlink ref="F40" r:id="rId454" xr:uid="{D92E6C55-67A9-4E1C-AD34-811C029D7666}"/>
+    <hyperlink ref="F39" r:id="rId455" xr:uid="{6DDE1B1B-14D4-4E76-81BD-640FFDBDEFE1}"/>
+    <hyperlink ref="F21" r:id="rId456" xr:uid="{C533FC1E-F228-4DBF-9788-03C422F7D4B1}"/>
+    <hyperlink ref="F16" r:id="rId457" xr:uid="{DDAB7A69-2818-48A3-920B-842DE9BEEBEF}"/>
+    <hyperlink ref="F303" r:id="rId458" xr:uid="{477E7E05-0F90-41CC-AC25-3E5BACABE644}"/>
+    <hyperlink ref="F306" r:id="rId459" xr:uid="{5A36384D-42B3-4AF5-AD70-7144403C714E}"/>
+    <hyperlink ref="F316" r:id="rId460" xr:uid="{1EEF5289-C2AB-4D6F-9A49-B1BED6347851}"/>
+    <hyperlink ref="F322" r:id="rId461" xr:uid="{674CB3A4-78EF-44D3-B4CD-9474022ED336}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId447"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId462"/>
 </worksheet>
 </file>
</xml_diff>